<commit_message>
sua 1 so bug trong file Update neu mario chet se tu dong ko va cham voi obj khac update neu an nam mang se tang mang
</commit_message>
<xml_diff>
--- a/LogBug/Bug_03-12-2015.xlsx
+++ b/LogBug/Bug_03-12-2015.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Introduction to Game development\ProjectMario\LogBug\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Bug</t>
   </si>
@@ -32,22 +27,10 @@
     <t>Case</t>
   </si>
   <si>
-    <t>tự biến nhỏ lại rồi biến lớn</t>
-  </si>
-  <si>
-    <t>Mario ăn nấm lần 2</t>
-  </si>
-  <si>
     <t>Chân mario chạm đỉnh của cây</t>
   </si>
   <si>
     <t>không xảy ra va chạm</t>
-  </si>
-  <si>
-    <t>Mario lớn chết(do lọt hố)</t>
-  </si>
-  <si>
-    <t>không xét lại size(render mario nhỏ nhưng dùng size mario lớn)</t>
   </si>
   <si>
     <t>Nấm sinh ra</t>
@@ -389,7 +372,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -400,7 +383,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,52 +400,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>